<commit_message>
display new bg color for stores to help
</commit_message>
<xml_diff>
--- a/06-30-24 to 07-06-24 Milwaukee Schedule Copy.xlsx
+++ b/06-30-24 to 07-06-24 Milwaukee Schedule Copy.xlsx
@@ -2034,8 +2034,16 @@
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Lashaun</t>
+        </is>
+      </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
@@ -2111,11 +2119,7 @@
       </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Office</t>
-        </is>
-      </c>
+      <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
@@ -2156,7 +2160,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Office</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
@@ -2185,7 +2189,11 @@
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>

</xml_diff>

<commit_message>
prep main for full schedule
</commit_message>
<xml_diff>
--- a/06-30-24 to 07-06-24 Milwaukee Schedule Copy.xlsx
+++ b/06-30-24 to 07-06-24 Milwaukee Schedule Copy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y61"/>
+  <dimension ref="A1:Y62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1260,7 +1260,7 @@
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
-          <t xml:space="preserve">7:00 AM START </t>
+          <t>Office</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
@@ -1311,7 +1311,7 @@
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
-          <t>EXCEL FINANCIAL</t>
+          <t>Lashaun</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
@@ -1344,11 +1344,7 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>DARIEN CORNER MART</t>
-        </is>
-      </c>
+      <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
@@ -1391,11 +1387,7 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>101 W. BELOIT ST</t>
-        </is>
-      </c>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
@@ -1443,11 +1435,7 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/Gx2Xk97tzdZtteHR8</t>
-        </is>
-      </c>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
@@ -1533,21 +1521,9 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>DJ</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>Equip</t>
-        </is>
-      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
@@ -1600,16 +1576,8 @@
         </is>
       </c>
       <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>Ian</t>
-        </is>
-      </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
@@ -1755,11 +1723,7 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>Office</t>
-        </is>
-      </c>
+      <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
@@ -1798,11 +1762,7 @@
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>Lashaun</t>
-        </is>
-      </c>
+      <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
@@ -2074,9 +2034,21 @@
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Lashaun</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Check In After Store</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
@@ -2151,11 +2123,7 @@
       </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Office</t>
-        </is>
-      </c>
+      <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
@@ -2196,7 +2164,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Office</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
@@ -2225,7 +2193,11 @@
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
@@ -2966,6 +2938,45 @@
       <c r="X61" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>7)</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Lashaun</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>After Store</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="inlineStr"/>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="inlineStr"/>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr"/>
+      <c r="Y62" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
do not display #
</commit_message>
<xml_diff>
--- a/06-30-24 to 07-06-24 Milwaukee Schedule Copy.xlsx
+++ b/06-30-24 to 07-06-24 Milwaukee Schedule Copy.xlsx
@@ -2034,8 +2034,16 @@
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Lashaun</t>
+        </is>
+      </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
@@ -2111,11 +2119,7 @@
       </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Office</t>
-        </is>
-      </c>
+      <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
@@ -2156,7 +2160,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Office</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
@@ -2185,7 +2189,11 @@
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>

</xml_diff>